<commit_message>
parse txt-files with our type of comments and markers for column names. new documentation for new data - not included.
</commit_message>
<xml_diff>
--- a/documentation.xlsx
+++ b/documentation.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pfsulliv/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Media\work\eclipse\TIEFighter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15980" tabRatio="500"/>
+    <workbookView xWindow="645" yWindow="1185" windowWidth="28155" windowHeight="15975" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -371,6 +368,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -641,28 +641,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>42393</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>42514</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -671,7 +673,7 @@
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -688,7 +690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -705,12 +707,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1">
-        <v>42375</v>
+        <v>42514</v>
       </c>
       <c r="C7" s="2">
         <v>22955987</v>
@@ -722,12 +724,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1">
-        <v>42321</v>
+        <v>42513</v>
       </c>
       <c r="C8" s="2">
         <v>24316577</v>
@@ -739,7 +741,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -756,7 +758,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -773,12 +775,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="1">
-        <v>42321</v>
+        <v>42513</v>
       </c>
       <c r="C11" s="2">
         <v>18842627</v>
@@ -790,7 +792,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -807,19 +809,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>33</v>
       </c>
@@ -830,7 +832,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -841,7 +843,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -852,7 +854,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -863,7 +865,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -874,7 +876,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5</v>
       </c>
@@ -885,14 +887,14 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>33</v>
       </c>
@@ -903,7 +905,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -914,7 +916,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -925,7 +927,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -936,7 +938,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4</v>
       </c>
@@ -947,7 +949,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
@@ -958,7 +960,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>6</v>
       </c>
@@ -969,7 +971,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7</v>
       </c>
@@ -980,7 +982,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>8</v>
       </c>
@@ -991,7 +993,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>9</v>
       </c>
@@ -1002,14 +1004,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>56</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>33</v>
       </c>
@@ -1020,7 +1022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1031,7 +1033,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1042,7 +1044,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -1053,7 +1055,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4</v>
       </c>
@@ -1064,7 +1066,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5</v>
       </c>
@@ -1075,7 +1077,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>6</v>
       </c>
@@ -1086,7 +1088,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>7</v>
       </c>
@@ -1097,14 +1099,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>65</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>33</v>
       </c>
@@ -1115,7 +1117,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -1126,7 +1128,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2</v>
       </c>
@@ -1137,7 +1139,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -1148,7 +1150,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4</v>
       </c>
@@ -1159,7 +1161,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>5</v>
       </c>
@@ -1170,14 +1172,14 @@
         <v>66</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>67</v>
       </c>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>33</v>
       </c>
@@ -1188,7 +1190,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1</v>
       </c>
@@ -1199,7 +1201,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2</v>
       </c>
@@ -1210,7 +1212,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>3</v>
       </c>
@@ -1221,7 +1223,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>4</v>
       </c>
@@ -1232,7 +1234,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>5</v>
       </c>
@@ -1243,7 +1245,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>6</v>
       </c>
@@ -1254,14 +1256,14 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>72</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>33</v>
       </c>
@@ -1272,7 +1274,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1</v>
       </c>
@@ -1283,7 +1285,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2</v>
       </c>
@@ -1294,7 +1296,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>3</v>
       </c>
@@ -1305,7 +1307,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>4</v>
       </c>
@@ -1316,7 +1318,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>5</v>
       </c>
@@ -1327,7 +1329,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>6</v>
       </c>
@@ -1338,7 +1340,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>7</v>
       </c>
@@ -1349,14 +1351,14 @@
         <v>77</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>78</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>33</v>
       </c>
@@ -1367,7 +1369,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1</v>
       </c>
@@ -1378,7 +1380,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2</v>
       </c>
@@ -1389,7 +1391,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>3</v>
       </c>
@@ -1400,7 +1402,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>4</v>
       </c>
@@ -1411,7 +1413,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>5</v>
       </c>
@@ -1422,7 +1424,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
documentation. output folder same as folder of input file as standard.
fixed bug.

temp folder setting from output setting (which might come from input
setting)

readme.md
</commit_message>
<xml_diff>
--- a/documentation.xlsx
+++ b/documentation.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="84">
   <si>
-    <t>PGC bioinformatics, PF Sullivan &amp; Johan Kallberg, Karolinska Institutet, (c) 2016</t>
-  </si>
-  <si>
     <t>Metadata for Bioinformatic Sources</t>
   </si>
   <si>
@@ -276,6 +273,9 @@
   </si>
   <si>
     <t>additional description</t>
+  </si>
+  <si>
+    <t>PGC bioinformatics, PF Sullivan &amp; JA Källberg Zvrskovec, Karolinska Institutet, (c) 2016</t>
   </si>
 </sst>
 </file>
@@ -642,7 +642,7 @@
   <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -656,7 +656,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -666,7 +666,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -675,41 +675,41 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>42372</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1">
         <v>42514</v>
@@ -718,15 +718,15 @@
         <v>22955987</v>
       </c>
       <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
         <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
         <v>42513</v>
@@ -735,32 +735,32 @@
         <v>24316577</v>
       </c>
       <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
         <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
         <v>42195</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1">
         <v>40722</v>
@@ -769,15 +769,15 @@
         <v>26578600</v>
       </c>
       <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
         <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1">
         <v>42513</v>
@@ -786,50 +786,50 @@
         <v>18842627</v>
       </c>
       <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
         <v>25</v>
-      </c>
-      <c r="E11" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1">
         <v>42393</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
         <v>28</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>29</v>
-      </c>
-      <c r="E12" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="C17" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -837,10 +837,10 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
         <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -848,10 +848,10 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
         <v>37</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -859,10 +859,10 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
         <v>39</v>
-      </c>
-      <c r="C20" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -870,10 +870,10 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
         <v>41</v>
-      </c>
-      <c r="C21" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -881,28 +881,28 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
         <v>43</v>
-      </c>
-      <c r="C22" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="C25" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -910,10 +910,10 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
         <v>35</v>
-      </c>
-      <c r="C26" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -921,10 +921,10 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" t="s">
         <v>37</v>
-      </c>
-      <c r="C27" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -932,10 +932,10 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" t="s">
         <v>39</v>
-      </c>
-      <c r="C28" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -943,10 +943,10 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
         <v>41</v>
-      </c>
-      <c r="C29" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -954,10 +954,10 @@
         <v>5</v>
       </c>
       <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" t="s">
         <v>46</v>
-      </c>
-      <c r="C30" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -965,10 +965,10 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
         <v>48</v>
-      </c>
-      <c r="C31" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -976,10 +976,10 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" t="s">
         <v>50</v>
-      </c>
-      <c r="C32" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -987,10 +987,10 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" t="s">
         <v>52</v>
-      </c>
-      <c r="C33" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -998,28 +998,28 @@
         <v>9</v>
       </c>
       <c r="B34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" t="s">
         <v>54</v>
-      </c>
-      <c r="C34" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="C37" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1027,10 +1027,10 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" t="s">
         <v>35</v>
-      </c>
-      <c r="C38" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1038,10 +1038,10 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" t="s">
         <v>37</v>
-      </c>
-      <c r="C39" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1049,10 +1049,10 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" t="s">
         <v>39</v>
-      </c>
-      <c r="C40" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1060,10 +1060,10 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" t="s">
         <v>57</v>
-      </c>
-      <c r="C41" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1071,10 +1071,10 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" t="s">
         <v>59</v>
-      </c>
-      <c r="C42" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1082,10 +1082,10 @@
         <v>6</v>
       </c>
       <c r="B43" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" t="s">
         <v>61</v>
-      </c>
-      <c r="C43" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1093,28 +1093,28 @@
         <v>7</v>
       </c>
       <c r="B44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" t="s">
         <v>63</v>
-      </c>
-      <c r="C44" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="C47" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1122,10 +1122,10 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" t="s">
         <v>35</v>
-      </c>
-      <c r="C48" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1133,10 +1133,10 @@
         <v>2</v>
       </c>
       <c r="B49" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" t="s">
         <v>37</v>
-      </c>
-      <c r="C49" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1144,10 +1144,10 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" t="s">
         <v>39</v>
-      </c>
-      <c r="C50" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1155,10 +1155,10 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" t="s">
         <v>41</v>
-      </c>
-      <c r="C51" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1166,28 +1166,28 @@
         <v>5</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C52" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="C55" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1195,10 +1195,10 @@
         <v>1</v>
       </c>
       <c r="B56" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56" t="s">
         <v>35</v>
-      </c>
-      <c r="C56" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1206,10 +1206,10 @@
         <v>2</v>
       </c>
       <c r="B57" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" t="s">
         <v>37</v>
-      </c>
-      <c r="C57" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1217,10 +1217,10 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" t="s">
         <v>39</v>
-      </c>
-      <c r="C58" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1228,10 +1228,10 @@
         <v>4</v>
       </c>
       <c r="B59" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" t="s">
         <v>41</v>
-      </c>
-      <c r="C59" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1239,10 +1239,10 @@
         <v>5</v>
       </c>
       <c r="B60" t="s">
+        <v>67</v>
+      </c>
+      <c r="C60" t="s">
         <v>68</v>
-      </c>
-      <c r="C60" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1250,28 +1250,28 @@
         <v>6</v>
       </c>
       <c r="B61" t="s">
+        <v>69</v>
+      </c>
+      <c r="C61" t="s">
         <v>70</v>
-      </c>
-      <c r="C61" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B64" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="C64" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1279,10 +1279,10 @@
         <v>1</v>
       </c>
       <c r="B65" t="s">
+        <v>34</v>
+      </c>
+      <c r="C65" t="s">
         <v>35</v>
-      </c>
-      <c r="C65" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1290,10 +1290,10 @@
         <v>2</v>
       </c>
       <c r="B66" t="s">
+        <v>36</v>
+      </c>
+      <c r="C66" t="s">
         <v>37</v>
-      </c>
-      <c r="C66" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1301,10 +1301,10 @@
         <v>3</v>
       </c>
       <c r="B67" t="s">
+        <v>38</v>
+      </c>
+      <c r="C67" t="s">
         <v>39</v>
-      </c>
-      <c r="C67" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1312,10 +1312,10 @@
         <v>4</v>
       </c>
       <c r="B68" t="s">
+        <v>40</v>
+      </c>
+      <c r="C68" t="s">
         <v>41</v>
-      </c>
-      <c r="C68" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1323,10 +1323,10 @@
         <v>5</v>
       </c>
       <c r="B69" t="s">
+        <v>72</v>
+      </c>
+      <c r="C69" t="s">
         <v>73</v>
-      </c>
-      <c r="C69" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1334,10 +1334,10 @@
         <v>6</v>
       </c>
       <c r="B70" t="s">
+        <v>74</v>
+      </c>
+      <c r="C70" t="s">
         <v>75</v>
-      </c>
-      <c r="C70" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1345,28 +1345,28 @@
         <v>7</v>
       </c>
       <c r="B71" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C71" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B74" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B74" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="C74" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1374,10 +1374,10 @@
         <v>1</v>
       </c>
       <c r="B75" t="s">
+        <v>34</v>
+      </c>
+      <c r="C75" t="s">
         <v>35</v>
-      </c>
-      <c r="C75" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1385,10 +1385,10 @@
         <v>2</v>
       </c>
       <c r="B76" t="s">
+        <v>36</v>
+      </c>
+      <c r="C76" t="s">
         <v>37</v>
-      </c>
-      <c r="C76" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1396,10 +1396,10 @@
         <v>3</v>
       </c>
       <c r="B77" t="s">
+        <v>38</v>
+      </c>
+      <c r="C77" t="s">
         <v>39</v>
-      </c>
-      <c r="C77" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1407,10 +1407,10 @@
         <v>4</v>
       </c>
       <c r="B78" t="s">
+        <v>78</v>
+      </c>
+      <c r="C78" t="s">
         <v>79</v>
-      </c>
-      <c r="C78" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -1418,10 +1418,10 @@
         <v>5</v>
       </c>
       <c r="B79" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C79" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1429,10 +1429,10 @@
         <v>6</v>
       </c>
       <c r="B80" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80" t="s">
         <v>82</v>
-      </c>
-      <c r="C80" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>